<commit_message>
model-a: something changed in the spreadsheet I guess
</commit_message>
<xml_diff>
--- a/model-a.xlsx
+++ b/model-a.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cimes/papers/2023-pmbs-opera-dlrm-eval/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6F2FD9-4E1E-5C4D-9242-6DD022F10850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9CC28D-DF9F-E641-A8C3-C7805C3710F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4180" yWindow="1560" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{DEAFE38A-293F-7042-BF18-6E0DF8B980B3}"/>
+    <workbookView xWindow="4160" yWindow="1560" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{DEAFE38A-293F-7042-BF18-6E0DF8B980B3}"/>
   </bookViews>
   <sheets>
     <sheet name="baseline" sheetId="1" r:id="rId1"/>

</xml_diff>